<commit_message>
Parallel test case is added
</commit_message>
<xml_diff>
--- a/src/main/java/com/makemytrip/testdata/TestSuite1.xlsx
+++ b/src/main/java/com/makemytrip/testdata/TestSuite1.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Steps" sheetId="2" r:id="rId2"/>
     <sheet name="Test Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="130">
   <si>
     <t>TCID</t>
   </si>
@@ -399,10 +400,13 @@
     <t>NYC</t>
   </si>
   <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
 </sst>
 </file>
@@ -814,12 +818,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="54.85546875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -898,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2267,7 +2271,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E33" r:id="rId8"/>
+    <hyperlink ref="E33" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2277,19 +2281,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="22.42578125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="32.140625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="18.87724609375" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.51728515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2410,7 +2415,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>37</v>
@@ -2422,7 +2427,7 @@
         <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2465,7 +2470,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
@@ -2484,6 +2489,9 @@
       </c>
       <c r="G13" t="s">
         <v>73</v>
+      </c>
+      <c r="H13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2505,10 +2513,13 @@
       <c r="G14" t="s">
         <v>55</v>
       </c>
+      <c r="H14" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>56</v>
@@ -2525,10 +2536,13 @@
       <c r="G15" t="s">
         <v>59</v>
       </c>
+      <c r="H15" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
@@ -2545,10 +2559,13 @@
       <c r="G16" t="s">
         <v>61</v>
       </c>
+      <c r="H16" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
         <v>60</v>
@@ -2566,6 +2583,9 @@
       <c r="G17" t="s">
         <v>63</v>
       </c>
+      <c r="H17" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
@@ -2587,10 +2607,13 @@
       <c r="G18" t="s">
         <v>66</v>
       </c>
+      <c r="H18" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
@@ -2610,10 +2633,13 @@
       <c r="G19" t="s">
         <v>68</v>
       </c>
+      <c r="H19" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>60</v>
@@ -2633,21 +2659,38 @@
       <c r="G20" t="s">
         <v>69</v>
       </c>
+      <c r="H20" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId78"/>
-    <hyperlink ref="B9" r:id="rId79"/>
-    <hyperlink ref="C9" r:id="rId80"/>
-    <hyperlink ref="E13" r:id="rId81"/>
-    <hyperlink ref="D9" r:id="rId82"/>
-    <hyperlink ref="E14" r:id="rId83"/>
-    <hyperlink ref="E15" r:id="rId84"/>
-    <hyperlink ref="E17" r:id="rId85"/>
-    <hyperlink ref="E19" r:id="rId86"/>
-    <hyperlink ref="E18" r:id="rId87"/>
-    <hyperlink ref="E20" r:id="rId88"/>
+    <hyperlink ref="E13" r:id="rId166"/>
+    <hyperlink ref="B4" r:id="rId167"/>
+    <hyperlink ref="B9" r:id="rId168"/>
+    <hyperlink ref="C9" r:id="rId169"/>
+    <hyperlink ref="D9" r:id="rId170"/>
+    <hyperlink ref="E14" r:id="rId171"/>
+    <hyperlink ref="E15" r:id="rId172"/>
+    <hyperlink ref="E17" r:id="rId173"/>
+    <hyperlink ref="E19" r:id="rId174"/>
+    <hyperlink ref="E18" r:id="rId175"/>
+    <hyperlink ref="E20" r:id="rId176"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>